<commit_message>
docs: Clarify the remark about the ADC pins maximum voltage.
</commit_message>
<xml_diff>
--- a/docs/PinOUT.xlsx
+++ b/docs/PinOUT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
   <si>
     <t>AF6</t>
   </si>
@@ -357,13 +357,28 @@
   </si>
   <si>
     <t>I2C_SDA[1]</t>
+  </si>
+  <si>
+    <t>Kwaliteit en leverbetrouwbaarheid zijn speerpunten in onze stamperij, dat is namelijk wat onze veeleisende klanten in de automotive, food, baby care, HVAC, Electronics, medical &amp; life sciences eisen.</t>
+  </si>
+  <si>
+    <t>Wanneer de nauwkeurigheden hoog, en de toleranties klein zijn, is de beschikbaarheid van de interne engineering en gereedschapmakerij een enorm voordeel. We identificeren problemen direct, en pakken ze snel aan. Bij de opstart van nieuwe produkten en tussentijdse wijzigingen komen we op dezelfde methode tot een alternatieve oplossing.</t>
+  </si>
+  <si>
+    <t>In onze stamperij hebben we excenter stansautomaten van 5 tot 160 ton, excenter C-frame persen van 25 tot 125 voor handinleg werk en automatisering, alsook enkele hydraulische persen. De produkten welke we maken lopen qua grootte uit elkaar van een speldekopje tot een schoenendoos, in dikte van 0,03 mm tot 6 mm. We verwerken een breed scala aan materialen, waaronder Ferro (staal, RVS, Cr-staal) Koper en zijn legeringen als messing, brons en nieuwzilver, als ook lichtmetalen als Aluminium, magnesium en titaan, maar ook exoten als zuiver nikkel en zuiver molybdeen.</t>
+  </si>
+  <si>
+    <t>Produkten kunnen losgestort, aan band, of in magazijnen afgeleverd worden. Seriegroottes van enkele losse stuks tot miljoenen.</t>
+  </si>
+  <si>
+    <t>We beschikken in de stamperij over een wasmachine en roto-finish equipment om de producten reinigen. Wij kunnen uw produkten eventueel ook nog mechanisch voor U samenstellen of eventueel puntlassen.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,6 +408,12 @@
       <sz val="9"/>
       <color indexed="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -552,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -604,6 +625,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,25 +698,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>7620</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="868680" y="3299460"/>
-          <a:ext cx="5295900" cy="609600"/>
+          <a:off x="7620" y="3291840"/>
+          <a:ext cx="5417820" cy="990600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -751,7 +773,10 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:pPr lvl="0"/>
+          <a:pPr marL="171450" lvl="0" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100" i="1">
               <a:solidFill>
@@ -762,7 +787,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>- The number next to each function is the one to be used when remapping the pin.</a:t>
+            <a:t>The number next to each function is the one to be used when remapping the pin.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
@@ -775,7 +800,10 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:pPr lvl="0"/>
+          <a:pPr marL="171450" lvl="0" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100" i="1">
               <a:solidFill>
@@ -786,7 +814,19 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>- ADC pin input range is 0-1.4V (being 1.8V the absolute maximum that it can withstand).</a:t>
+            <a:t>ADC pin input range is 0-1.4V (being 1.8V the absolute maximum that it can withstand).  If  GPIO2, GPIO3, GPIO4 or GPIO5 are remapped</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> to the ADC block, 1.8 V is the maximum. If these pins are used in digital mode, then the maximum allowed input is 3.6V.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
@@ -1071,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:O21"/>
+  <dimension ref="A3:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1601,6 +1641,34 @@
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I21" s="1"/>
     </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K28" s="21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K30" s="21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K32" s="21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K34" s="21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K35" s="21"/>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K36" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="12" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
docs: Update pinout to show the board orientation.
</commit_message>
<xml_diff>
--- a/docs/PinOUT.xlsx
+++ b/docs/PinOUT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
   <si>
     <t>AF6</t>
   </si>
@@ -53,9 +53,6 @@
     <t>RESET</t>
   </si>
   <si>
-    <t>VIN</t>
-  </si>
-  <si>
     <t>ADC_CH0</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>GPIO1</t>
   </si>
   <si>
-    <t>3V3</t>
-  </si>
-  <si>
     <t>GPIO23</t>
   </si>
   <si>
@@ -372,13 +366,22 @@
   </si>
   <si>
     <t>We beschikken in de stamperij over een wasmachine en roto-finish equipment om de producten reinigen. Wij kunnen uw produkten eventueel ook nog mechanisch voor U samenstellen of eventueel puntlassen.</t>
+  </si>
+  <si>
+    <t>Antenna</t>
+  </si>
+  <si>
+    <t>VIN (3.6-5.5V)</t>
+  </si>
+  <si>
+    <t>3V3 OUT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,8 +419,16 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,6 +516,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF9966FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -624,8 +641,10 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,62 +670,18 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>50018</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>99065</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1699699</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>92589</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="5023377" y="1008346"/>
-          <a:ext cx="2370964" cy="1649681"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>701040</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -715,8 +690,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7620" y="3291840"/>
-          <a:ext cx="5417820" cy="990600"/>
+          <a:off x="2796540" y="4046220"/>
+          <a:ext cx="5585460" cy="990600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -724,7 +699,7 @@
         <a:solidFill>
           <a:schemeClr val="lt1"/>
         </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
+        <a:ln w="12700" cmpd="sng">
           <a:solidFill>
             <a:schemeClr val="lt1">
               <a:shade val="50000"/>
@@ -751,7 +726,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1">
+            <a:rPr lang="en-US" sz="1200" b="1">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -762,7 +737,7 @@
             </a:rPr>
             <a:t>Remarks:</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
+          <a:endParaRPr lang="en-US" sz="1200">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
             </a:solidFill>
@@ -814,7 +789,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>ADC pin input range is 0-1.4V (being 1.8V the absolute maximum that it can withstand).  If  GPIO2, GPIO3, GPIO4 or GPIO5 are remapped</a:t>
+            <a:t>ADC pin input range is 0-1.4V (being 1.8V the absolute maximum that it can withstand). When GPIO2, GPIO3, GPIO4 or GPIO5 are remapped</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" i="1" baseline="0">
@@ -840,6 +815,146 @@
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>20502</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1728493</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>107450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4398363" y="978999"/>
+          <a:ext cx="2401070" cy="1707991"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3162300" y="22860"/>
+          <a:ext cx="4869180" cy="312420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="12700" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" i="0" u="sng">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>WiPy</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" i="0" u="sng" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> pinout and alternate functions table</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800" b="1" i="0" u="sng">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1800" b="1" i="0" u="sng">
+            <a:latin typeface="+mn-lt"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1111,137 +1226,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:O36"/>
+  <dimension ref="A5:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="1" max="5" width="9.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" customWidth="1"/>
     <col min="8" max="8" width="25.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
     <col min="10" max="10" width="10.6640625" customWidth="1"/>
-    <col min="11" max="15" width="10" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="15" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="16"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="15"/>
       <c r="I6" s="18" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1253,420 +1316,478 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>64</v>
+      <c r="C7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H7" s="16"/>
-      <c r="I7" s="8" t="s">
-        <v>16</v>
+      <c r="I7" s="19" t="s">
+        <v>11</v>
       </c>
       <c r="J7" s="3"/>
-      <c r="K7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>52</v>
-      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="10" t="s">
-        <v>68</v>
-      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>66</v>
+        <v>80</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H8" s="16"/>
-      <c r="I8" s="8" t="s">
-        <v>18</v>
+      <c r="I8" s="18" t="s">
+        <v>116</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="O8" s="11" t="s">
-        <v>105</v>
-      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>84</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="9" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="K9" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="L9" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="11" t="s">
-        <v>63</v>
+        <v>89</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>42</v>
-      </c>
+      <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="D10" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>43</v>
+        <v>65</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="L10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
+      <c r="M10" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>102</v>
+      </c>
       <c r="O10" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="D11" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>53</v>
+        <v>108</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>96</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
       <c r="L11" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
+      <c r="O11" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>54</v>
+      <c r="A12" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="G12" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>76</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
       <c r="O12" s="11" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="G13" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="N13" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="O13" s="11" t="s">
-        <v>109</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>57</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="5" t="s">
-        <v>61</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="5" t="s">
-        <v>62</v>
-      </c>
+      <c r="D15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="3"/>
       <c r="G15" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>93</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="L15" s="3"/>
       <c r="M15" s="13" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="N15" s="11" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="O15" s="11" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="3"/>
+      <c r="A16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="G16" s="8" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="A17" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="17"/>
+      <c r="I19" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="M19" s="3"/>
+      <c r="N19" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="M17" s="3"/>
-      <c r="N17" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
+    </row>
+    <row r="20" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H20" s="21" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I21" s="1"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K28" s="21" t="s">
+      <c r="K28" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K30" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K32" s="20" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K30" s="21" t="s">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K34" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K32" s="21" t="s">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K35" s="20"/>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K36" s="20" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K34" s="21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K35" s="21"/>
-    </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K36" s="21" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: Update PinOUT table with Timer CC and PWM pins.
</commit_message>
<xml_diff>
--- a/docs/PinOUT.xlsx
+++ b/docs/PinOUT.xlsx
@@ -24,25 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
-  <si>
-    <t>AF6</t>
-  </si>
-  <si>
-    <t>AF5</t>
-  </si>
-  <si>
-    <t>AF4</t>
-  </si>
-  <si>
-    <t>AF3</t>
-  </si>
-  <si>
-    <t>AF2</t>
-  </si>
-  <si>
-    <t>AF1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="134">
   <si>
     <t>PIN</t>
   </si>
@@ -53,9 +35,6 @@
     <t>RESET</t>
   </si>
   <si>
-    <t>ADC_CH0</t>
-  </si>
-  <si>
     <t>GPIO2</t>
   </si>
   <si>
@@ -375,13 +354,85 @@
   </si>
   <si>
     <t>3V3 OUT</t>
+  </si>
+  <si>
+    <t>Timer</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>TIM_CC0</t>
+  </si>
+  <si>
+    <t>TIM_CC1</t>
+  </si>
+  <si>
+    <t>TIM_CC2</t>
+  </si>
+  <si>
+    <t>TIM_CC3</t>
+  </si>
+  <si>
+    <t>TIM_CC4</t>
+  </si>
+  <si>
+    <t>TIM_CC5</t>
+  </si>
+  <si>
+    <t>TIM_CC6</t>
+  </si>
+  <si>
+    <t>TIM_CC7</t>
+  </si>
+  <si>
+    <t>PWM_CH0</t>
+  </si>
+  <si>
+    <t>PWM_CH2</t>
+  </si>
+  <si>
+    <t>PWM_CH5</t>
+  </si>
+  <si>
+    <t>PWM_CH6</t>
+  </si>
+  <si>
+    <t>PWM_CH7</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>CC pin</t>
+  </si>
+  <si>
+    <t>PWM pin</t>
+  </si>
+  <si>
+    <t>ADC_CH4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,8 +478,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,6 +606,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -590,12 +683,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -627,9 +717,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -643,6 +730,30 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -672,16 +783,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -690,8 +801,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2796540" y="4046220"/>
-          <a:ext cx="5585460" cy="990600"/>
+          <a:off x="4686300" y="4312920"/>
+          <a:ext cx="5737860" cy="1478280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -762,7 +873,19 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>The number next to each function is the one to be used when remapping the pin.</a:t>
+            <a:t>The number in brackets next to each function is the one to be used when remapping the pin.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> In order to use the pin in GPIO mode, alternate function 0 must be selected</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
@@ -803,15 +926,24 @@
             </a:rPr>
             <a:t> to the ADC block, 1.8 V is the maximum. If these pins are used in digital mode, then the maximum allowed input is 3.6V.</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" lvl="0" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The heart beat LED is connected to GPIO25 and also has PWM_CH2 functionality with the alternate function 9.</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
@@ -1226,569 +1358,715 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:O36"/>
+  <dimension ref="A5:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="9.77734375" customWidth="1"/>
+    <col min="1" max="3" width="9.77734375" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" customWidth="1"/>
     <col min="8" max="8" width="25.44140625" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
     <col min="10" max="10" width="10.6640625" customWidth="1"/>
-    <col min="11" max="11" width="10.5546875" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" customWidth="1"/>
     <col min="13" max="15" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="H5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="I5" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="H6" s="13"/>
+      <c r="I6" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="H7" s="14"/>
+      <c r="I7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H8" s="14"/>
+      <c r="I8" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H9" s="14"/>
+      <c r="I9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4" t="s">
+      <c r="J9" s="2"/>
+      <c r="K9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="5" t="s">
+      <c r="H10" s="14"/>
+      <c r="I10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="6" t="s">
+      <c r="E15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="9" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="N9" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O9" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="O17" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="15"/>
+      <c r="I19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O10" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="N14" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="O14" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="N15" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="O15" s="11" t="s">
+      <c r="O19" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H20" s="19" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="16"/>
-      <c r="I17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="M17" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="N17" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="O17" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="M19" s="3"/>
-      <c r="N19" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O19" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H20" s="21" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I21" s="1"/>
     </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B24" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B25" s="23">
+        <v>1</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B26" s="22"/>
+      <c r="C26" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="22"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B27" s="23">
+        <v>2</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>123</v>
+      </c>
+    </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K28" s="20" t="s">
-        <v>109</v>
-      </c>
+      <c r="B28" s="22"/>
+      <c r="C28" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="22"/>
+      <c r="K28" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B29" s="23">
+        <v>3</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="23"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K30" s="20" t="s">
-        <v>110</v>
+      <c r="B30" s="22"/>
+      <c r="C30" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="K30" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="20"/>
+      <c r="B31" s="23">
+        <v>4</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K32" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K34" s="20" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K35" s="20"/>
-    </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K36" s="20" t="s">
+      <c r="A32" s="21"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="24" t="s">
         <v>113</v>
       </c>
+      <c r="D32" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="K32" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="K34" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="K35" s="18"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="K36" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
docs: Rename pins from GPIO to GP.
</commit_message>
<xml_diff>
--- a/docs/PinOUT.xlsx
+++ b/docs/PinOUT.xlsx
@@ -35,90 +35,18 @@
     <t>RESET</t>
   </si>
   <si>
-    <t>GPIO2</t>
-  </si>
-  <si>
     <t>GND</t>
   </si>
   <si>
-    <t>GPIO1</t>
-  </si>
-  <si>
-    <t>GPIO23</t>
-  </si>
-  <si>
-    <t>GPIO10</t>
-  </si>
-  <si>
-    <t>GPIO24</t>
-  </si>
-  <si>
-    <t>GPIO9</t>
-  </si>
-  <si>
-    <t>GPIO11</t>
-  </si>
-  <si>
-    <t>GPIO8</t>
-  </si>
-  <si>
-    <t>GPIO12</t>
-  </si>
-  <si>
-    <t>GPIO7</t>
-  </si>
-  <si>
-    <t>GPIO13</t>
-  </si>
-  <si>
-    <t>GPIO6</t>
-  </si>
-  <si>
-    <t>GPIO14</t>
-  </si>
-  <si>
-    <t>GPIO30</t>
-  </si>
-  <si>
-    <t>GPIO15</t>
-  </si>
-  <si>
-    <t>GPIO31</t>
-  </si>
-  <si>
-    <t>GPIO16</t>
-  </si>
-  <si>
-    <t>GPIO3</t>
-  </si>
-  <si>
     <t>ADC_CH1</t>
   </si>
   <si>
-    <t>GPIO17</t>
-  </si>
-  <si>
-    <t>GPIO0</t>
-  </si>
-  <si>
-    <t>GPIO22</t>
-  </si>
-  <si>
-    <t>GPIO4</t>
-  </si>
-  <si>
     <t>ADC_CH2</t>
   </si>
   <si>
     <t>SAFE_BOOT</t>
   </si>
   <si>
-    <t>GPIO28</t>
-  </si>
-  <si>
-    <t>GPIO5</t>
-  </si>
-  <si>
     <t>ADC_CH3</t>
   </si>
   <si>
@@ -426,6 +354,78 @@
   </si>
   <si>
     <t>ADC_CH4</t>
+  </si>
+  <si>
+    <t>GP2</t>
+  </si>
+  <si>
+    <t>GP1</t>
+  </si>
+  <si>
+    <t>GP23</t>
+  </si>
+  <si>
+    <t>GP24</t>
+  </si>
+  <si>
+    <t>GP11</t>
+  </si>
+  <si>
+    <t>GP12</t>
+  </si>
+  <si>
+    <t>GP13</t>
+  </si>
+  <si>
+    <t>GP14</t>
+  </si>
+  <si>
+    <t>GP15</t>
+  </si>
+  <si>
+    <t>GP16</t>
+  </si>
+  <si>
+    <t>GP17</t>
+  </si>
+  <si>
+    <t>GP22</t>
+  </si>
+  <si>
+    <t>GP28</t>
+  </si>
+  <si>
+    <t>GP10</t>
+  </si>
+  <si>
+    <t>GP9</t>
+  </si>
+  <si>
+    <t>GP8</t>
+  </si>
+  <si>
+    <t>GP7</t>
+  </si>
+  <si>
+    <t>GP6</t>
+  </si>
+  <si>
+    <t>GP30</t>
+  </si>
+  <si>
+    <t>GP31</t>
+  </si>
+  <si>
+    <t>GP3</t>
+  </si>
+  <si>
+    <t>GP0</t>
+  </si>
+  <si>
+    <t>GP4</t>
+  </si>
+  <si>
+    <t>GP5</t>
   </si>
 </sst>
 </file>
@@ -912,7 +912,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>ADC pin input range is 0-1.4V (being 1.8V the absolute maximum that it can withstand). When GPIO2, GPIO3, GPIO4 or GPIO5 are remapped</a:t>
+            <a:t>ADC pin input range is 0-1.4V (being 1.8V the absolute maximum that it can withstand). When GP2, GP3, GP4 or GP5 are remapped</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" i="1" baseline="0">
@@ -942,7 +942,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>The heart beat LED is connected to GPIO25 and also has PWM_CH2 functionality with the alternate function 9.</a:t>
+            <a:t>The heart beat LED is connected to GP25 and also has PWM_CH2 functionality with the alternate function 9.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -955,15 +955,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>20502</xdr:colOff>
+      <xdr:colOff>43950</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>117232</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1728493</xdr:colOff>
+      <xdr:colOff>1711234</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>107450</xdr:rowOff>
+      <xdr:rowOff>84001</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -986,8 +986,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="4398363" y="978999"/>
-          <a:ext cx="2401070" cy="1707991"/>
+          <a:off x="4384753" y="1356613"/>
+          <a:ext cx="2328969" cy="1667284"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1360,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1381,22 +1381,22 @@
   <sheetData>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="G5" s="25" t="s">
         <v>0</v>
@@ -1408,22 +1408,22 @@
         <v>0</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="K5" s="25" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="L5" s="25" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="M5" s="25" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="N5" s="25" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="O5" s="25" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="16" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1451,23 +1451,23 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>3</v>
+        <v>110</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1481,20 +1481,20 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="5" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="16" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1509,144 +1509,144 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="8" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="7" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="9" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="7" t="s">
-        <v>9</v>
+        <v>124</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="5" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="7" t="s">
-        <v>11</v>
+        <v>125</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="5" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="10" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="5" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="7" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="10" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -1654,29 +1654,29 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="5" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="7" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1684,179 +1684,179 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="5" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="7" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="7" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="5" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="5" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="7" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="7" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="12" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="O15" s="10" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="5" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="4" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="7" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="4" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="4" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="4" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="7" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
       <c r="J17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="M17" s="12" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="O17" s="10" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="5" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="7" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="H18" s="14"/>
       <c r="I18" s="7" t="s">
-        <v>26</v>
+        <v>132</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="4" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="4" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -1866,31 +1866,31 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>29</v>
+        <v>122</v>
       </c>
       <c r="H19" s="15"/>
       <c r="I19" s="7" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="5" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="10" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H20" s="19" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -1898,16 +1898,16 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B24" s="27" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -1915,22 +1915,22 @@
         <v>1</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B26" s="22"/>
       <c r="C26" s="24" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="E26" s="22"/>
     </row>
@@ -1939,26 +1939,26 @@
         <v>2</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B28" s="22"/>
       <c r="C28" s="24" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="E28" s="22"/>
       <c r="K28" s="18" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -1966,26 +1966,26 @@
         <v>3</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="E29" s="23"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B30" s="22"/>
       <c r="C30" s="24" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="K30" s="18" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -1994,29 +1994,29 @@
         <v>4</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="21"/>
       <c r="B32" s="22"/>
       <c r="C32" s="24" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="K32" s="18" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -2031,7 +2031,7 @@
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
       <c r="K34" s="18" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -2047,7 +2047,7 @@
       <c r="C36" s="21"/>
       <c r="D36" s="21"/>
       <c r="K36" s="18" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
docs: Update pin out to reflect the new API.
</commit_message>
<xml_diff>
--- a/docs/PinOUT.xlsx
+++ b/docs/PinOUT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VirtualBoxShared\GitHub\wipy\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\310150182\Github\wipy\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="PinOUT" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="129">
   <si>
     <t>PIN</t>
   </si>
@@ -44,27 +44,9 @@
     <t>UART1_RX[7]</t>
   </si>
   <si>
-    <t>SD_CMD[6]</t>
-  </si>
-  <si>
     <t>UART1_TX[7]</t>
   </si>
   <si>
-    <t>SD_CLK[6]</t>
-  </si>
-  <si>
-    <t>I2C_SCL[1]</t>
-  </si>
-  <si>
-    <t>SD_DATA0[8]</t>
-  </si>
-  <si>
-    <t>SD_CLK[8]</t>
-  </si>
-  <si>
-    <t>SD_CMD[8]</t>
-  </si>
-  <si>
     <t>UART1_RTS[10]</t>
   </si>
   <si>
@@ -104,24 +86,6 @@
     <t>TIM_CC6[12]</t>
   </si>
   <si>
-    <t>SD_DATA0[6]</t>
-  </si>
-  <si>
-    <t>Kwaliteit en leverbetrouwbaarheid zijn speerpunten in onze stamperij, dat is namelijk wat onze veeleisende klanten in de automotive, food, baby care, HVAC, Electronics, medical &amp; life sciences eisen.</t>
-  </si>
-  <si>
-    <t>Wanneer de nauwkeurigheden hoog, en de toleranties klein zijn, is de beschikbaarheid van de interne engineering en gereedschapmakerij een enorm voordeel. We identificeren problemen direct, en pakken ze snel aan. Bij de opstart van nieuwe produkten en tussentijdse wijzigingen komen we op dezelfde methode tot een alternatieve oplossing.</t>
-  </si>
-  <si>
-    <t>In onze stamperij hebben we excenter stansautomaten van 5 tot 160 ton, excenter C-frame persen van 25 tot 125 voor handinleg werk en automatisering, alsook enkele hydraulische persen. De produkten welke we maken lopen qua grootte uit elkaar van een speldekopje tot een schoenendoos, in dikte van 0,03 mm tot 6 mm. We verwerken een breed scala aan materialen, waaronder Ferro (staal, RVS, Cr-staal) Koper en zijn legeringen als messing, brons en nieuwzilver, als ook lichtmetalen als Aluminium, magnesium en titaan, maar ook exoten als zuiver nikkel en zuiver molybdeen.</t>
-  </si>
-  <si>
-    <t>Produkten kunnen losgestort, aan band, of in magazijnen afgeleverd worden. Seriegroottes van enkele losse stuks tot miljoenen.</t>
-  </si>
-  <si>
-    <t>We beschikken in de stamperij over een wasmachine en roto-finish equipment om de producten reinigen. Wij kunnen uw produkten eventueel ook nog mechanisch voor U samenstellen of eventueel puntlassen.</t>
-  </si>
-  <si>
     <t>Antenna</t>
   </si>
   <si>
@@ -254,57 +218,9 @@
     <t>GP5</t>
   </si>
   <si>
-    <t>UART2_TX[2]</t>
-  </si>
-  <si>
-    <t>UART2_RX[2]</t>
-  </si>
-  <si>
-    <t>UART2_RX[7]</t>
-  </si>
-  <si>
-    <t>UART2_TX[5]</t>
-  </si>
-  <si>
-    <t>UART2_RX[5]</t>
-  </si>
-  <si>
-    <t>UART2_RX[6]</t>
-  </si>
-  <si>
-    <t>UART2_TX[6]</t>
-  </si>
-  <si>
-    <t>UART2_TX[7]</t>
-  </si>
-  <si>
-    <t>UART2_RTS[3]</t>
-  </si>
-  <si>
-    <t>UART2_CTS[3]</t>
-  </si>
-  <si>
-    <t>UART2_RTS[10]</t>
-  </si>
-  <si>
-    <t>UART1_RX[3]</t>
-  </si>
-  <si>
-    <t>UART1_TX[3]</t>
-  </si>
-  <si>
     <t>UART1_TX[11]</t>
   </si>
   <si>
-    <t>UART1_CTS[6]</t>
-  </si>
-  <si>
-    <t>UART1_TX[9]</t>
-  </si>
-  <si>
-    <t>UART1_RX[9]</t>
-  </si>
-  <si>
     <t>TIM_CC8</t>
   </si>
   <si>
@@ -353,79 +269,148 @@
     <t>TIM_CC3[7]</t>
   </si>
   <si>
-    <t>ADC1_CH1</t>
-  </si>
-  <si>
-    <t>ADC1_CH2</t>
-  </si>
-  <si>
-    <t>ADC1_CH3</t>
-  </si>
-  <si>
-    <t>ADC1_CH4</t>
-  </si>
-  <si>
-    <t>I2S1_FS[13]</t>
-  </si>
-  <si>
-    <t>I2S1_CLK[3]</t>
-  </si>
-  <si>
-    <t>SPI1_CLK[7]</t>
-  </si>
-  <si>
-    <t>SPI1_MISO[7]</t>
-  </si>
-  <si>
-    <t>SPI1_MOSI[7]</t>
-  </si>
-  <si>
-    <t>SPI1_CS[7]</t>
-  </si>
-  <si>
-    <t>I2S1_FS[7]</t>
-  </si>
-  <si>
-    <t>I2C1_SCL[9]</t>
-  </si>
-  <si>
-    <t>I2C1_SDA[9]</t>
-  </si>
-  <si>
-    <t>I2C1_SDA[1]</t>
-  </si>
-  <si>
-    <t>I2C1_SCL[5]</t>
-  </si>
-  <si>
-    <t>I2C1_SDA[5]</t>
-  </si>
-  <si>
-    <t>SPI1_CS[9]</t>
-  </si>
-  <si>
-    <t>I2S1_FS[3]</t>
-  </si>
-  <si>
-    <t>I2S1_FS[12]</t>
-  </si>
-  <si>
-    <t>I2S1_DATA0[4]</t>
-  </si>
-  <si>
-    <t>I2S1_DATA1[6]</t>
-  </si>
-  <si>
-    <t>I2S1_DATA0[7]</t>
-  </si>
-  <si>
-    <t>I2S1_CLK[13]</t>
-  </si>
-  <si>
-    <t>I2S1_CLK[2]</t>
-  </si>
-  <si>
-    <t>I2S1_DAT0[6]</t>
+    <t>I2S0_FS[13]</t>
+  </si>
+  <si>
+    <t>I2S0_CLK[3]</t>
+  </si>
+  <si>
+    <t>SPI0_CLK[7]</t>
+  </si>
+  <si>
+    <t>SPI0_MISO[7]</t>
+  </si>
+  <si>
+    <t>SPI0_MOSI[7]</t>
+  </si>
+  <si>
+    <t>SPI0_CS[7]</t>
+  </si>
+  <si>
+    <t>I2S0_FS[7]</t>
+  </si>
+  <si>
+    <t>SD0_CMD[6]</t>
+  </si>
+  <si>
+    <t>SD0_DATA0[8]</t>
+  </si>
+  <si>
+    <t>SD0_CLK[8]</t>
+  </si>
+  <si>
+    <t>SD0_CMD[8]</t>
+  </si>
+  <si>
+    <t>ADC0_CH0</t>
+  </si>
+  <si>
+    <t>UART1_RX[6]</t>
+  </si>
+  <si>
+    <t>UART1_TX[6]</t>
+  </si>
+  <si>
+    <t>I2C0_SCL[9]</t>
+  </si>
+  <si>
+    <t>I2C0_SDA[9]</t>
+  </si>
+  <si>
+    <t>I2C0_SDA[1]</t>
+  </si>
+  <si>
+    <t>I2C0_SCL[5]</t>
+  </si>
+  <si>
+    <t>I2C0_SDA[5]</t>
+  </si>
+  <si>
+    <t>UART0_RX[3]</t>
+  </si>
+  <si>
+    <t>UART0_TX[3]</t>
+  </si>
+  <si>
+    <t>UART1_TX[2]</t>
+  </si>
+  <si>
+    <t>UART1_RX[2]</t>
+  </si>
+  <si>
+    <t>UART0_TX[7]</t>
+  </si>
+  <si>
+    <t>UART0_RX[7]</t>
+  </si>
+  <si>
+    <t>UART1_TX[5]</t>
+  </si>
+  <si>
+    <t>UART1_RX[5]</t>
+  </si>
+  <si>
+    <t>UART0_RTS[10]</t>
+  </si>
+  <si>
+    <t>UART0_CTS[6]</t>
+  </si>
+  <si>
+    <t>UART0_TX[9]</t>
+  </si>
+  <si>
+    <t>UART0_RX[9]</t>
+  </si>
+  <si>
+    <t>UART0_RTS[3]</t>
+  </si>
+  <si>
+    <t>UART1_CTS[3]</t>
+  </si>
+  <si>
+    <t>SPI0_CS[9]</t>
+  </si>
+  <si>
+    <t>SD0_CLK[6]</t>
+  </si>
+  <si>
+    <t>SD0_DATA0[6]</t>
+  </si>
+  <si>
+    <t>I2S0_FS[3]</t>
+  </si>
+  <si>
+    <t>I2S0_FS[12]</t>
+  </si>
+  <si>
+    <t>I2S0_DATA0[4]</t>
+  </si>
+  <si>
+    <t>I2S0_DATA1[6]</t>
+  </si>
+  <si>
+    <t>I2C0_SCL[1]</t>
+  </si>
+  <si>
+    <t>I2S0_DATA0[7]</t>
+  </si>
+  <si>
+    <t>I2S0_CLK[13]</t>
+  </si>
+  <si>
+    <t>I2S0_CLK[2]</t>
+  </si>
+  <si>
+    <t>I2S0_DAT0[6]</t>
+  </si>
+  <si>
+    <t>ADC0_CH1</t>
+  </si>
+  <si>
+    <t>ADC0_CH2</t>
+  </si>
+  <si>
+    <t>ADC0_CH3</t>
   </si>
 </sst>
 </file>
@@ -489,19 +474,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8.5"/>
+      <sz val="10"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="8.5"/>
+      <sz val="10"/>
       <color indexed="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="8.5"/>
+      <sz val="10"/>
       <color indexed="9"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -718,9 +703,15 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -733,6 +724,9 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -748,19 +742,10 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -962,13 +947,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>43950</xdr:colOff>
+      <xdr:colOff>24900</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>117232</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1711234</xdr:colOff>
+      <xdr:colOff>1673134</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>84001</xdr:rowOff>
     </xdr:to>
@@ -993,8 +978,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="4384753" y="1356613"/>
-          <a:ext cx="2328969" cy="1667284"/>
+          <a:off x="4632770" y="1462487"/>
+          <a:ext cx="2433744" cy="1648234"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1367,46 +1352,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection sqref="A1:O33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" customWidth="1"/>
-    <col min="8" max="8" width="25.44140625" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" customWidth="1"/>
-    <col min="11" max="11" width="10.5546875" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" customWidth="1"/>
-    <col min="14" max="15" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>0</v>
@@ -1418,661 +1404,651 @@
         <v>0</v>
       </c>
       <c r="J5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="11" t="s">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="N9" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="N10" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="O10" s="24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="K14" s="15"/>
+      <c r="L14" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="N14" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="O14" s="24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="L15" s="15"/>
+      <c r="M15" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="N15" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="O15" s="24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="15"/>
+      <c r="K16" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="N17" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="O17" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="J18" s="15"/>
+      <c r="K18" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="M19" s="15"/>
+      <c r="N19" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H20" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="G7" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="N9" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="O9" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="N10" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="O10" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="21" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="J12" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="L12" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="K13" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="J14" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="K14" s="14"/>
-      <c r="L14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M14" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="N14" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="O14" s="21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="K15" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="L15" s="14"/>
-      <c r="M15" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="N15" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="O15" s="21" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="J16" s="14"/>
-      <c r="K16" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="J17" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="L17" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="M17" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="N17" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="O17" s="21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="J18" s="14"/>
-      <c r="K18" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M19" s="14"/>
-      <c r="N19" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="O19" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="H20" s="28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="I21" s="1"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B24" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>50</v>
-      </c>
       <c r="E24" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" s="9">
         <v>1</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" s="10" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" s="9">
         <v>2</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
       <c r="C28" s="10" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E28" s="8"/>
-      <c r="K28" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K28" s="5"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" s="9">
         <v>3</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="10" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="9">
         <v>4</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="8"/>
       <c r="C32" s="10" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="K32" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
-      <c r="K34" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="K35" s="5"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
-      <c r="K36" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -2080,7 +2056,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="12" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: Update PinOUT to reflect new Timer IDs.
</commit_message>
<xml_diff>
--- a/docs/PinOUT.xlsx
+++ b/docs/PinOUT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\310150182\Github\wipy\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\wipy\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
   <si>
     <t>PIN</t>
   </si>
@@ -50,42 +50,9 @@
     <t>UART1_RTS[10]</t>
   </si>
   <si>
-    <t>TIM_CC2[7]</t>
-  </si>
-  <si>
-    <t>TIM_CC1[7]</t>
-  </si>
-  <si>
-    <t>TIM_CC6[4]</t>
-  </si>
-  <si>
-    <t>TIM_CC2[12]</t>
-  </si>
-  <si>
-    <t>TIM_CC3[12]</t>
-  </si>
-  <si>
-    <t>TIM_CC4[12]</t>
-  </si>
-  <si>
-    <t>TIM_CC5[12]</t>
-  </si>
-  <si>
-    <t>TIM_CC7[13]</t>
-  </si>
-  <si>
-    <t>TIM_CC1[12]</t>
-  </si>
-  <si>
-    <t>TIM_CC6[7]</t>
-  </si>
-  <si>
     <t>UART1_RTS[3]</t>
   </si>
   <si>
-    <t>TIM_CC6[12]</t>
-  </si>
-  <si>
     <t>Antenna</t>
   </si>
   <si>
@@ -107,27 +74,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>TIM_CC1</t>
-  </si>
-  <si>
-    <t>TIM_CC2</t>
-  </si>
-  <si>
-    <t>TIM_CC3</t>
-  </si>
-  <si>
-    <t>TIM_CC4</t>
-  </si>
-  <si>
-    <t>TIM_CC5</t>
-  </si>
-  <si>
-    <t>TIM_CC6</t>
-  </si>
-  <si>
-    <t>TIM_CC7</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -140,9 +86,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>CC pin</t>
-  </si>
-  <si>
     <t>PWM pin</t>
   </si>
   <si>
@@ -221,9 +164,6 @@
     <t>UART1_TX[11]</t>
   </si>
   <si>
-    <t>TIM_CC8</t>
-  </si>
-  <si>
     <t>PWM_1</t>
   </si>
   <si>
@@ -249,24 +189,6 @@
   </si>
   <si>
     <t>PWM_6[3]</t>
-  </si>
-  <si>
-    <t>TIM_CC7[7]</t>
-  </si>
-  <si>
-    <t>TIM_CC7[12]</t>
-  </si>
-  <si>
-    <t>TIM_CC5[5]</t>
-  </si>
-  <si>
-    <t>TIM_CC8[13]</t>
-  </si>
-  <si>
-    <t>TIM_CC7[4]</t>
-  </si>
-  <si>
-    <t>TIM_CC3[7]</t>
   </si>
   <si>
     <t>I2S0_FS[13]</t>
@@ -492,7 +414,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -574,12 +496,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="30"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9966FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -672,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -685,13 +601,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -703,7 +619,7 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -712,10 +628,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1352,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,22 +1290,22 @@
   <sheetData>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>0</v>
@@ -1404,22 +1317,22 @@
         <v>0</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1433,8 +1346,8 @@
         <v>2</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="27" t="s">
-        <v>21</v>
+      <c r="I6" s="26" t="s">
+        <v>10</v>
       </c>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
@@ -1447,22 +1360,20 @@
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>40</v>
+        <v>66</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="H7" s="3"/>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="27" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="15"/>
@@ -1476,21 +1387,19 @@
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
-      <c r="D8" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>41</v>
+      <c r="D8" s="15"/>
+      <c r="E8" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="H8" s="3"/>
-      <c r="I8" s="27" t="s">
-        <v>22</v>
+      <c r="I8" s="26" t="s">
+        <v>11</v>
       </c>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -1504,355 +1413,327 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="15"/>
+      <c r="M9" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="N9" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="O9" s="21" t="s">
         <v>95</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="N9" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="O9" s="22" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="15"/>
-      <c r="C10" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>43</v>
+      <c r="C10" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="H10" s="3"/>
-      <c r="I10" s="21" t="s">
-        <v>54</v>
+      <c r="I10" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
-      <c r="L10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="N10" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="O10" s="24" t="s">
-        <v>122</v>
+      <c r="L10" s="15"/>
+      <c r="M10" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="N10" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="O10" s="23" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="19" t="s">
+      <c r="A11" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="21" t="s">
-        <v>44</v>
+      <c r="G11" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="21" t="s">
-        <v>55</v>
+      <c r="I11" s="20" t="s">
+        <v>36</v>
       </c>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
-      <c r="L11" s="18" t="s">
-        <v>76</v>
-      </c>
+      <c r="L11" s="15"/>
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
-      <c r="O11" s="24" t="s">
-        <v>87</v>
+      <c r="O11" s="23" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>82</v>
+      <c r="A12" s="23" t="s">
+        <v>56</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
-      <c r="D12" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="21" t="s">
+      <c r="D12" s="15"/>
+      <c r="E12" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="19" t="s">
         <v>45</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="J12" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" s="20" t="s">
-        <v>64</v>
       </c>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
-      <c r="O12" s="24" t="s">
-        <v>123</v>
+      <c r="O12" s="23" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
-      <c r="D13" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>46</v>
+      <c r="D13" s="15"/>
+      <c r="E13" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="I13" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="L13" s="15"/>
       <c r="M13" s="15"/>
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>83</v>
+      <c r="A14" s="25" t="s">
+        <v>57</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="22" t="s">
+      <c r="D14" s="15"/>
+      <c r="E14" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="N14" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="O14" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="21" t="s">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="J14" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="K14" s="15"/>
-      <c r="L14" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="M14" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="N14" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="O14" s="24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>89</v>
+      <c r="B15" s="24" t="s">
+        <v>63</v>
       </c>
       <c r="C15" s="15"/>
-      <c r="D15" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="22" t="s">
+      <c r="D15" s="15"/>
+      <c r="E15" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="L15" s="15"/>
+      <c r="M15" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="O15" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="21" t="s">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="K15" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="L15" s="15"/>
-      <c r="M15" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="N15" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="O15" s="24" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>90</v>
+      <c r="B16" s="24" t="s">
+        <v>64</v>
       </c>
       <c r="C16" s="15"/>
-      <c r="D16" s="18" t="s">
-        <v>78</v>
-      </c>
+      <c r="D16" s="15"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>49</v>
+      <c r="F16" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="I16" s="21" t="s">
-        <v>60</v>
+      <c r="I16" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="J16" s="15"/>
-      <c r="K16" s="19" t="s">
-        <v>94</v>
+      <c r="K16" s="18" t="s">
+        <v>68</v>
       </c>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
       <c r="N16" s="15"/>
       <c r="O16" s="17" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>91</v>
+      <c r="A17" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>65</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
-      <c r="F17" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>50</v>
+      <c r="F17" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>31</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17" s="21" t="s">
+      <c r="I17" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="L17" s="15"/>
+      <c r="M17" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="N17" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="O17" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
         <v>61</v>
-      </c>
-      <c r="J17" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="K17" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="L17" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="M17" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="N17" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="O17" s="24" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
-        <v>87</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
-      <c r="D18" s="18" t="s">
-        <v>77</v>
-      </c>
+      <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="21" t="s">
-        <v>51</v>
+      <c r="G18" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="H18" s="3"/>
-      <c r="I18" s="21" t="s">
-        <v>62</v>
+      <c r="I18" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="J18" s="15"/>
-      <c r="K18" s="19" t="s">
-        <v>93</v>
+      <c r="K18" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
       <c r="N18" s="15"/>
       <c r="O18" s="17" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1864,29 +1745,27 @@
       <c r="F19" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="21" t="s">
-        <v>52</v>
+      <c r="G19" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="H19" s="4"/>
-      <c r="I19" s="21" t="s">
-        <v>63</v>
+      <c r="I19" s="20" t="s">
+        <v>44</v>
       </c>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
-      <c r="L19" s="18" t="s">
-        <v>17</v>
-      </c>
+      <c r="L19" s="15"/>
       <c r="M19" s="15"/>
-      <c r="N19" s="24" t="s">
-        <v>120</v>
+      <c r="N19" s="23" t="s">
+        <v>94</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H20" s="14" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1894,118 +1773,91 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" s="13" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="D26" s="8"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
       <c r="C28" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="D28" s="8"/>
       <c r="K28" s="5"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="10" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="8"/>
       <c r="C32" s="10" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="K32" s="5"/>
     </row>

</xml_diff>